<commit_message>
Velmi dobrá shoda reakcí
</commit_message>
<xml_diff>
--- a/WindDataProcessing/TestovaciData/vysledky_testovani.xlsx
+++ b/WindDataProcessing/TestovaciData/vysledky_testovani.xlsx
@@ -12,11 +12,12 @@
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>PRJ-6076_DLC24_OVS_V11.0_N_S1_FATIGUE</t>
   </si>
@@ -384,19 +385,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -415,16 +416,16 @@
       <c r="E1" s="1">
         <v>620161.396227333</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>389</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>263</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>4202</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <f>SUM(F1:H1)</f>
         <v>4854</v>
       </c>
@@ -448,13 +449,13 @@
       <c r="E2" s="1">
         <v>630759.75264424703</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>389</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>263</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>4202</v>
       </c>
       <c r="M2" t="s">
@@ -477,19 +478,19 @@
       <c r="E3" s="1">
         <v>668698.46432052006</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>389</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>263</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>4202</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>140</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
       <c r="K3">
@@ -502,6 +503,41 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2104401.16788114</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1233079.4681556099</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1401312.69478258</v>
+      </c>
+      <c r="E5" s="1">
+        <v>748528.80624845705</v>
+      </c>
+      <c r="F5">
+        <v>386</v>
+      </c>
+      <c r="G5">
+        <v>267</v>
+      </c>
+      <c r="H5">
+        <v>4201</v>
+      </c>
+      <c r="I5">
+        <v>140</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>